<commit_message>
update produc collect permission, add fucntion check_collect download ,produc collect download
</commit_message>
<xml_diff>
--- a/src/main/resources/templet/upload/askcost.xlsx
+++ b/src/main/resources/templet/upload/askcost.xlsx
@@ -16,22 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>询价单位</t>
-  </si>
-  <si>
-    <t>询价人</t>
-  </si>
-  <si>
-    <t>询价日期</t>
-  </si>
-  <si>
-    <t>报价人</t>
-  </si>
-  <si>
-    <t>报价日期</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>商品名称</t>
   </si>
@@ -55,13 +40,41 @@
   </si>
   <si>
     <t>客户利润总价</t>
+  </si>
+  <si>
+    <t>客户</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>计划员</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单下达日期</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>技术条件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZGC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +96,14 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -128,12 +149,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,14 +463,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="3" max="3" width="16.625" customWidth="1"/>
+    <col min="5" max="5" width="17.625" customWidth="1"/>
     <col min="8" max="8" width="24.25" customWidth="1"/>
     <col min="11" max="11" width="20.375" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
@@ -451,44 +480,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3">
+        <v>43415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>